<commit_message>
move to new pc
</commit_message>
<xml_diff>
--- a/0_data/three_challenges_codebook.xlsx
+++ b/0_data/three_challenges_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clemens Lindner\Documents\github\bigot_and_tolerant_personalites\0_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F2EB33-A0BF-462E-9ADB-27B2396F0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66987F3-87FD-4AD9-AD2D-863785AC12F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5059903E-ADBB-4520-B1A6-60D4EA1E22CC}"/>
+    <workbookView xWindow="-38520" yWindow="-2025" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{5059903E-ADBB-4520-B1A6-60D4EA1E22CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Study 1a" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="726">
   <si>
     <t>variable</t>
   </si>
@@ -2503,6 +2503,183 @@
   </si>
   <si>
     <t>Highest level of education, ES - ISCED</t>
+  </si>
+  <si>
+    <t>education_eisced</t>
+  </si>
+  <si>
+    <t>trad_1</t>
+  </si>
+  <si>
+    <t>trad_2</t>
+  </si>
+  <si>
+    <t>trad_3</t>
+  </si>
+  <si>
+    <t>trad_4</t>
+  </si>
+  <si>
+    <t>trad_5</t>
+  </si>
+  <si>
+    <t>trad_6</t>
+  </si>
+  <si>
+    <t>prj_immi_1</t>
+  </si>
+  <si>
+    <t>prj_immi_2</t>
+  </si>
+  <si>
+    <t>prj_immi_3</t>
+  </si>
+  <si>
+    <t>prj_immi_4</t>
+  </si>
+  <si>
+    <t>prj_immi_5</t>
+  </si>
+  <si>
+    <t>prj_gay_1</t>
+  </si>
+  <si>
+    <t>prj_wmn_1</t>
+  </si>
+  <si>
+    <t>prj_wmn_2</t>
+  </si>
+  <si>
+    <t>prj_unempl_1</t>
+  </si>
+  <si>
+    <t>prj_age20</t>
+  </si>
+  <si>
+    <t>prj_age70</t>
+  </si>
+  <si>
+    <t>ess4</t>
+  </si>
+  <si>
+    <t>ess7</t>
+  </si>
+  <si>
+    <t>ess8</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>ess_variable_name</t>
+  </si>
+  <si>
+    <t>Prejudice_jews</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>prj_jews</t>
+  </si>
+  <si>
+    <t>aljewlv</t>
+  </si>
+  <si>
+    <t>Allow many or few Jewish people to come and live in country</t>
+  </si>
+  <si>
+    <t>Allow many or few Muslims to come and live in country</t>
+  </si>
+  <si>
+    <t>Prejudice_muslims</t>
+  </si>
+  <si>
+    <t>prj_muslms</t>
+  </si>
+  <si>
+    <t>almuslv</t>
+  </si>
+  <si>
+    <t>algyplv</t>
+  </si>
+  <si>
+    <t>prj_sinti</t>
+  </si>
+  <si>
+    <t>Prejudice_sinti_roma</t>
+  </si>
+  <si>
+    <t>Allow many or few Gypsies to come and live in country</t>
+  </si>
+  <si>
+    <t>alpfpe</t>
+  </si>
+  <si>
+    <t>Allow professionals from [poor European country providing largest number of migrants]</t>
+  </si>
+  <si>
+    <t>Prejudice_poorer_countries</t>
+  </si>
+  <si>
+    <t>Allow professionals from [poor non-European country providing largest number of migrants]</t>
+  </si>
+  <si>
+    <t>alpfpne</t>
+  </si>
+  <si>
+    <t>prj_prf_poor_2</t>
+  </si>
+  <si>
+    <t>prj_prf_poor_1</t>
+  </si>
+  <si>
+    <t>Allow unskilled labourers from [poor European country providing largest number of migrants]</t>
+  </si>
+  <si>
+    <t>allbpe</t>
+  </si>
+  <si>
+    <t>prj_unsk_poor_1</t>
+  </si>
+  <si>
+    <t>Allow unskilled labourers from [poor non-European country providing largest number of migrants]</t>
+  </si>
+  <si>
+    <t>allbpne</t>
+  </si>
+  <si>
+    <t>prj_unsk_poor_2</t>
+  </si>
+  <si>
+    <t>gvslvue</t>
+  </si>
+  <si>
+    <t>prj_unempl_2</t>
+  </si>
+  <si>
+    <t>dfincac</t>
+  </si>
+  <si>
+    <t>prj_unempl_3</t>
+  </si>
+  <si>
+    <t>bennent</t>
+  </si>
+  <si>
+    <t>prj_unempl_4</t>
+  </si>
+  <si>
+    <t>sblazy</t>
+  </si>
+  <si>
+    <t>prj_unempl_5</t>
+  </si>
+  <si>
+    <t>sbbsntx</t>
+  </si>
+  <si>
+    <t>prj_unempl_6</t>
   </si>
 </sst>
 </file>
@@ -7590,278 +7767,598 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4791DDA-356D-43C5-A405-960C4C715D9E}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="27.36328125" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>494</v>
+        <v>689</v>
       </c>
       <c r="B1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>495</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>522</v>
       </c>
+      <c r="B2" t="s">
+        <v>522</v>
+      </c>
       <c r="C2" t="s">
+        <v>688</v>
+      </c>
+      <c r="G2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>454</v>
       </c>
+      <c r="B3" t="s">
+        <v>586</v>
+      </c>
       <c r="C3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G3" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>456</v>
       </c>
+      <c r="B4" t="s">
+        <v>456</v>
+      </c>
       <c r="C4" t="s">
+        <v>688</v>
+      </c>
+      <c r="G4" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>458</v>
       </c>
+      <c r="B5" t="s">
+        <v>458</v>
+      </c>
       <c r="C5" t="s">
+        <v>688</v>
+      </c>
+      <c r="G5" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>665</v>
       </c>
+      <c r="B6" t="s">
+        <v>667</v>
+      </c>
       <c r="C6" t="s">
+        <v>688</v>
+      </c>
+      <c r="G6" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>496</v>
       </c>
+      <c r="B7" t="s">
+        <v>496</v>
+      </c>
       <c r="C7" t="s">
+        <v>688</v>
+      </c>
+      <c r="G7" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>498</v>
       </c>
+      <c r="B8" t="s">
+        <v>498</v>
+      </c>
       <c r="C8" t="s">
+        <v>688</v>
+      </c>
+      <c r="G8" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>460</v>
       </c>
       <c r="B9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C9" t="s">
+        <v>688</v>
+      </c>
+      <c r="F9" t="s">
         <v>141</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>462</v>
       </c>
       <c r="B10" t="s">
+        <v>669</v>
+      </c>
+      <c r="C10" t="s">
+        <v>688</v>
+      </c>
+      <c r="F10" t="s">
         <v>141</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>464</v>
       </c>
       <c r="B11" t="s">
+        <v>670</v>
+      </c>
+      <c r="C11" t="s">
+        <v>688</v>
+      </c>
+      <c r="F11" t="s">
         <v>141</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>466</v>
       </c>
       <c r="B12" t="s">
+        <v>671</v>
+      </c>
+      <c r="C12" t="s">
+        <v>688</v>
+      </c>
+      <c r="F12" t="s">
         <v>141</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>468</v>
       </c>
       <c r="B13" t="s">
+        <v>672</v>
+      </c>
+      <c r="C13" t="s">
+        <v>688</v>
+      </c>
+      <c r="F13" t="s">
         <v>141</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>470</v>
       </c>
       <c r="B14" t="s">
+        <v>673</v>
+      </c>
+      <c r="C14" t="s">
+        <v>688</v>
+      </c>
+      <c r="F14" t="s">
         <v>141</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>472</v>
       </c>
       <c r="B15" t="s">
+        <v>674</v>
+      </c>
+      <c r="C15" t="s">
+        <v>688</v>
+      </c>
+      <c r="F15" t="s">
         <v>517</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>474</v>
       </c>
       <c r="B16" t="s">
+        <v>675</v>
+      </c>
+      <c r="C16" t="s">
+        <v>688</v>
+      </c>
+      <c r="F16" t="s">
         <v>517</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>476</v>
       </c>
       <c r="B17" t="s">
+        <v>676</v>
+      </c>
+      <c r="C17" t="s">
+        <v>688</v>
+      </c>
+      <c r="F17" t="s">
         <v>517</v>
       </c>
-      <c r="C17" t="s">
+      <c r="G17" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>478</v>
       </c>
       <c r="B18" t="s">
+        <v>677</v>
+      </c>
+      <c r="C18" t="s">
+        <v>688</v>
+      </c>
+      <c r="F18" t="s">
         <v>517</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>480</v>
       </c>
       <c r="B19" t="s">
+        <v>678</v>
+      </c>
+      <c r="C19" t="s">
+        <v>688</v>
+      </c>
+      <c r="F19" t="s">
         <v>517</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>482</v>
       </c>
       <c r="B20" t="s">
+        <v>679</v>
+      </c>
+      <c r="C20" t="s">
+        <v>688</v>
+      </c>
+      <c r="F20" t="s">
         <v>515</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>484</v>
       </c>
       <c r="B21" t="s">
+        <v>680</v>
+      </c>
+      <c r="C21" t="s">
+        <v>688</v>
+      </c>
+      <c r="F21" t="s">
         <v>516</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>486</v>
       </c>
       <c r="B22" t="s">
+        <v>681</v>
+      </c>
+      <c r="C22" t="s">
+        <v>688</v>
+      </c>
+      <c r="F22" t="s">
         <v>516</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>488</v>
       </c>
       <c r="B23" t="s">
+        <v>682</v>
+      </c>
+      <c r="C23" t="s">
+        <v>688</v>
+      </c>
+      <c r="F23" t="s">
         <v>518</v>
       </c>
-      <c r="C23" t="s">
+      <c r="G23" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>490</v>
       </c>
       <c r="B24" t="s">
+        <v>683</v>
+      </c>
+      <c r="C24" t="s">
+        <v>688</v>
+      </c>
+      <c r="F24" t="s">
         <v>519</v>
       </c>
-      <c r="C24" t="s">
+      <c r="G24" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>492</v>
       </c>
       <c r="B25" t="s">
+        <v>684</v>
+      </c>
+      <c r="C25" t="s">
+        <v>688</v>
+      </c>
+      <c r="F25" t="s">
         <v>519</v>
       </c>
-      <c r="C25" t="s">
+      <c r="G25" t="s">
         <v>493</v>
       </c>
     </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>693</v>
+      </c>
+      <c r="B26" t="s">
+        <v>692</v>
+      </c>
+      <c r="C26" t="s">
+        <v>691</v>
+      </c>
+      <c r="F26" t="s">
+        <v>690</v>
+      </c>
+      <c r="G26" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>698</v>
+      </c>
+      <c r="B27" t="s">
+        <v>697</v>
+      </c>
+      <c r="C27" t="s">
+        <v>691</v>
+      </c>
+      <c r="F27" t="s">
+        <v>696</v>
+      </c>
+      <c r="G27" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>699</v>
+      </c>
+      <c r="B28" t="s">
+        <v>700</v>
+      </c>
+      <c r="C28" t="s">
+        <v>691</v>
+      </c>
+      <c r="F28" t="s">
+        <v>701</v>
+      </c>
+      <c r="G28" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>703</v>
+      </c>
+      <c r="B29" t="s">
+        <v>709</v>
+      </c>
+      <c r="C29" t="s">
+        <v>691</v>
+      </c>
+      <c r="F29" t="s">
+        <v>705</v>
+      </c>
+      <c r="G29" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>707</v>
+      </c>
+      <c r="B30" t="s">
+        <v>708</v>
+      </c>
+      <c r="C30" t="s">
+        <v>691</v>
+      </c>
+      <c r="F30" t="s">
+        <v>705</v>
+      </c>
+      <c r="G30" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>711</v>
+      </c>
+      <c r="B31" t="s">
+        <v>712</v>
+      </c>
+      <c r="C31" t="s">
+        <v>691</v>
+      </c>
+      <c r="F31" t="s">
+        <v>705</v>
+      </c>
+      <c r="G31" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>714</v>
+      </c>
+      <c r="B32" t="s">
+        <v>715</v>
+      </c>
+      <c r="C32" t="s">
+        <v>691</v>
+      </c>
+      <c r="F32" t="s">
+        <v>705</v>
+      </c>
+      <c r="G32" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>716</v>
+      </c>
+      <c r="B33" t="s">
+        <v>717</v>
+      </c>
+      <c r="F33" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>718</v>
+      </c>
+      <c r="B34" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>720</v>
+      </c>
+      <c r="B35" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>722</v>
+      </c>
+      <c r="B36" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>724</v>
+      </c>
+      <c r="B37" t="s">
+        <v>725</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>